<commit_message>
modifications on LOGIN TESTCASES
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_TC_LOGIN_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_TC_LOGIN_REVIEWS.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mego\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halae\OneDrive\Documents\GitHub\Group-3-Learning-hub\LH_REVIEWS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C8B31F-10AE-422F-B12F-26352D1A22BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{5AC26BFC-4949-4339-B766-2ABB4B88E1A8}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Version History" sheetId="1" r:id="rId1"/>
     <sheet name="Review sheet" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="57">
   <si>
     <t>Author</t>
   </si>
@@ -219,11 +218,14 @@
   <si>
     <t>the feature (new user? Sign up) button was not tested</t>
   </si>
+  <si>
+    <t>Closed</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -369,12 +371,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{83973D6D-C4A2-4DA6-8E86-0E47BD1D4D6C}" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{55AF0159-5A5D-4FB8-B45C-3CCBCD52D82E}" name="Version Number" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{A1BB0B96-5946-458D-A1EB-D1860A2E9A2C}" name="Author" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{7757C6A1-AD9C-489D-82AA-BCA0AEDC7F50}" name="Updated Section" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{484250C4-2243-4A67-B67B-4A70A88C9D78}" name="Date" dataDxfId="11">
+    <tableColumn id="1" name="Version Number" dataDxfId="14"/>
+    <tableColumn id="2" name="Author" dataDxfId="13"/>
+    <tableColumn id="3" name="Updated Section" dataDxfId="12"/>
+    <tableColumn id="4" name="Date" dataDxfId="11">
       <calculatedColumnFormula>DATE(2025,4,16)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -383,18 +385,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{24F4B5B1-870D-49D9-886C-D18ECE106044}" name="Table2" displayName="Table2" ref="A1:J31" totalsRowShown="0" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J31" totalsRowShown="0" dataDxfId="10">
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{154D141F-D70B-42BC-A41E-539A28623C91}" name="date" dataDxfId="9"/>
-    <tableColumn id="11" xr3:uid="{4302D07D-1297-4A5D-8113-2317E944B040}" name="Review ID" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{FBF8D811-3328-47BA-BC1D-3D576EA1DAB6}" name="Reviewed Entity" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{18FF139E-B651-4240-BB94-D9B167C69A0B}" name="Reviewer" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{B63C6CDA-7136-454D-9369-ADF32D470B5E}" name="Version" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{A3F78CBF-8865-4A12-B192-C2D9A7E27A67}" name="Review Comments" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{F15DDF96-B3DE-490B-B5E1-EA2B8996F9B7}" name="Actions" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{CD6623E7-579E-4453-B3EF-FB2A474583B7}" name="Owner" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{E5418A75-71B3-4C99-955B-196E2C83D64E}" name="Owner Status" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{FFFAAB40-2BF2-4CDE-A704-8DB308BED7C4}" name="Reviewer verification" dataDxfId="0"/>
+    <tableColumn id="1" name="date" dataDxfId="9"/>
+    <tableColumn id="11" name="Review ID" dataDxfId="8"/>
+    <tableColumn id="2" name="Reviewed Entity" dataDxfId="7"/>
+    <tableColumn id="3" name="Reviewer" dataDxfId="6"/>
+    <tableColumn id="4" name="Version" dataDxfId="5"/>
+    <tableColumn id="5" name="Review Comments" dataDxfId="4"/>
+    <tableColumn id="6" name="Actions" dataDxfId="3"/>
+    <tableColumn id="7" name="Owner" dataDxfId="2"/>
+    <tableColumn id="8" name="Owner Status" dataDxfId="1"/>
+    <tableColumn id="9" name="Reviewer verification" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -696,22 +698,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39D1DECC-CF93-47E4-94A2-AD404E424C77}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.109375" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" customWidth="1"/>
-    <col min="3" max="3" width="36.5546875" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="36.5703125" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -725,7 +727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
@@ -740,43 +742,43 @@
         <v>45763</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="9"/>
     </row>
-    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="9"/>
     </row>
-    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="9"/>
     </row>
-    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="9"/>
     </row>
-    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="9"/>
     </row>
-    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -791,27 +793,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{774AF0B9-8F49-46C8-8EB7-0F5E66F92113}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="D8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="43.6640625" customWidth="1"/>
-    <col min="6" max="6" width="39.88671875" customWidth="1"/>
-    <col min="7" max="7" width="32.6640625" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" customWidth="1"/>
-    <col min="9" max="9" width="19.5546875" customWidth="1"/>
+    <col min="5" max="5" width="43.7109375" customWidth="1"/>
+    <col min="6" max="6" width="39.85546875" customWidth="1"/>
+    <col min="7" max="7" width="32.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -843,7 +845,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="4" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="4" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <f>DATE(2025,4,16)</f>
         <v>45763</v>
@@ -870,14 +872,14 @@
         <v>3</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>26</v>
       </c>
       <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="1:11" s="3" customFormat="1" ht="144" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" s="3" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <f t="shared" ref="A3:A13" si="0">DATE(2025,4,16)</f>
         <v>45763</v>
@@ -904,14 +906,14 @@
         <v>3</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="J3" s="7" t="s">
         <v>26</v>
       </c>
       <c r="K3"/>
     </row>
-    <row r="4" spans="1:11" s="3" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
@@ -938,14 +940,14 @@
         <v>3</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="J4" s="7" t="s">
         <v>26</v>
       </c>
       <c r="K4"/>
     </row>
-    <row r="5" spans="1:11" s="3" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
@@ -972,14 +974,14 @@
         <v>3</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="J5" s="7" t="s">
         <v>26</v>
       </c>
       <c r="K5"/>
     </row>
-    <row r="6" spans="1:11" s="3" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
@@ -1006,14 +1008,14 @@
         <v>3</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="J6" s="7" t="s">
         <v>26</v>
       </c>
       <c r="K6"/>
     </row>
-    <row r="7" spans="1:11" s="3" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
@@ -1040,14 +1042,14 @@
         <v>3</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="J7" s="7" t="s">
         <v>26</v>
       </c>
       <c r="K7"/>
     </row>
-    <row r="8" spans="1:11" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
@@ -1074,14 +1076,14 @@
         <v>3</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="J8" s="7" t="s">
         <v>26</v>
       </c>
       <c r="K8"/>
     </row>
-    <row r="9" spans="1:11" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
@@ -1108,14 +1110,14 @@
         <v>3</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="J9" s="7" t="s">
         <v>26</v>
       </c>
       <c r="K9"/>
     </row>
-    <row r="10" spans="1:11" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
@@ -1142,14 +1144,14 @@
         <v>3</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="J10" s="7" t="s">
         <v>26</v>
       </c>
       <c r="K10"/>
     </row>
-    <row r="11" spans="1:11" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
@@ -1176,14 +1178,14 @@
         <v>3</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="J11" s="7" t="s">
         <v>26</v>
       </c>
       <c r="K11"/>
     </row>
-    <row r="12" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
@@ -1210,13 +1212,13 @@
         <v>3</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="J12" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
@@ -1243,13 +1245,13 @@
         <v>3</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="J13" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="13"/>
       <c r="C14" s="12"/>
@@ -1261,7 +1263,7 @@
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="B15" s="13"/>
       <c r="C15" s="12"/>
@@ -1273,7 +1275,7 @@
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="B16" s="13"/>
       <c r="C16" s="12"/>
@@ -1285,7 +1287,7 @@
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="13"/>
       <c r="C17" s="12"/>
@@ -1297,7 +1299,7 @@
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="13"/>
       <c r="C18" s="12"/>
@@ -1309,7 +1311,7 @@
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
@@ -1321,7 +1323,7 @@
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
@@ -1333,7 +1335,7 @@
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
@@ -1345,7 +1347,7 @@
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
@@ -1357,7 +1359,7 @@
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
@@ -1369,7 +1371,7 @@
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
@@ -1381,7 +1383,7 @@
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
@@ -1393,7 +1395,7 @@
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
@@ -1405,7 +1407,7 @@
       <c r="I26" s="12"/>
       <c r="J26" s="12"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
@@ -1417,7 +1419,7 @@
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
@@ -1429,7 +1431,7 @@
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
@@ -1441,7 +1443,7 @@
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
@@ -1453,7 +1455,7 @@
       <c r="I30" s="12"/>
       <c r="J30" s="12"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
@@ -1468,13 +1470,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H32:H1048576" xr:uid="{FDF361F9-8A76-4851-9C50-9A28BC1FE0CE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H32:H1048576">
       <formula1>"open,inProgress,notApplicable,close"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I31" xr:uid="{7106F391-5C30-4C5F-9FBD-F7D4EC019822}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I31">
       <formula1>"Open,InProgress,NotApplicable,Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J31" xr:uid="{A78E9E59-D51C-493A-A3EB-CA8CF067530D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J31">
       <formula1>"Open,Closed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
v1.1 Added crucial missing review points
LH_TC_LOGIN_Review_004
Added crucial missing review points regarding the TC_ID column and modified Filename review and Status and Actual result column
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_TC_LOGIN_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_TC_LOGIN_REVIEWS.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halae\OneDrive\Documents\GitHub\Group-3-Learning-hub\LH_REVIEWS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mego\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FEC51F6-FD26-411C-B8A9-22901276514B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5AC26BFC-4949-4339-B766-2ABB4B88E1A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Version History" sheetId="1" r:id="rId1"/>
     <sheet name="Review sheet" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="67">
   <si>
     <t>Author</t>
   </si>
@@ -117,18 +118,10 @@
   </si>
   <si>
     <t>Open</t>
-  </si>
-  <si>
-    <t>1-user is alread registered precondition is unnecessary
-2- there is no space between the username and the password in the test data column 
-3-in the steps column steps index number is mixed with the steps data because there are no spaces, bad redability</t>
   </si>
   <si>
     <t>1-there is no space between the username and the password in the test data column 
 2- in the steps column steps index number is mixed with the steps data because there are no spaces, bad redability</t>
-  </si>
-  <si>
-    <t>this feature is out of scope</t>
   </si>
   <si>
     <t>1-delete testcase because its out of scope</t>
@@ -201,12 +194,6 @@
     <t>1.0</t>
   </si>
   <si>
-    <t xml:space="preserve">File name is using - for spacing instead of _ </t>
-  </si>
-  <si>
-    <t>1-Change filename to follow the naming convention</t>
-  </si>
-  <si>
     <t>LH_REVIEW_TC_LOGIN_012</t>
   </si>
   <si>
@@ -216,16 +203,67 @@
     <t>1-include testcases to test this feature</t>
   </si>
   <si>
-    <t>the feature (new user? Sign up) button was not tested</t>
+    <t>LH_REVIEW_TC_LOGIN_013</t>
+  </si>
+  <si>
+    <t>TC_ID column</t>
+  </si>
+  <si>
+    <t>1-Replace the TC_ID column with SRS_ID for traceability means which includes the SRS ID that the TC is related to</t>
+  </si>
+  <si>
+    <t>1-This column is redundant because there is already an id column  
+2-the SRS_ID column is missing , which will be used for traceability</t>
+  </si>
+  <si>
+    <t>1-this feature is out of scope</t>
+  </si>
+  <si>
+    <t>1-the feature (new user? Sign up) button was not tested</t>
+  </si>
+  <si>
+    <t>v1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-File name is using - for spacing instead of _ 
+2-the word sheet is not necessary
+</t>
+  </si>
+  <si>
+    <t>1-Change filename to follow the naming convention
+2-Remove the word SHEET from the name</t>
+  </si>
+  <si>
+    <t>LH_REVIEW_TC_LOGIN_014</t>
   </si>
   <si>
     <t>Closed</t>
+  </si>
+  <si>
+    <t>1-There is no status and Acutual results column which are necessary for tc execution</t>
+  </si>
+  <si>
+    <t>1-user is already registered precondition is unnecessary
+2- there is no space between the username and the password in the test data column 
+3-in the steps column steps index number is mixed with the steps data because there are no spaces, bad redability</t>
+  </si>
+  <si>
+    <t>Status column
+and Acutal results
+column</t>
+  </si>
+  <si>
+    <t>1-Add Status column with 4 choices
+Pass,Fail,Blocked,Not executed and the default placeholder is Not executed</t>
+  </si>
+  <si>
+    <t>Added crucial missing review points regarding the TC_ID column and modified Filename review and Status and Actual result column</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -261,7 +299,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -294,49 +332,43 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
@@ -371,12 +403,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{83973D6D-C4A2-4DA6-8E86-0E47BD1D4D6C}" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <tableColumns count="4">
-    <tableColumn id="1" name="Version Number" dataDxfId="14"/>
-    <tableColumn id="2" name="Author" dataDxfId="13"/>
-    <tableColumn id="3" name="Updated Section" dataDxfId="12"/>
-    <tableColumn id="4" name="Date" dataDxfId="11">
+    <tableColumn id="1" xr3:uid="{55AF0159-5A5D-4FB8-B45C-3CCBCD52D82E}" name="Version Number" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{A1BB0B96-5946-458D-A1EB-D1860A2E9A2C}" name="Author" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{7757C6A1-AD9C-489D-82AA-BCA0AEDC7F50}" name="Updated Section" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{484250C4-2243-4A67-B67B-4A70A88C9D78}" name="Date" dataDxfId="11">
       <calculatedColumnFormula>DATE(2025,4,16)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -385,18 +417,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J31" totalsRowShown="0" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{24F4B5B1-870D-49D9-886C-D18ECE106044}" name="Table2" displayName="Table2" ref="A1:J31" totalsRowShown="0" dataDxfId="10">
   <tableColumns count="10">
-    <tableColumn id="1" name="date" dataDxfId="9"/>
-    <tableColumn id="11" name="Review ID" dataDxfId="8"/>
-    <tableColumn id="2" name="Reviewed Entity" dataDxfId="7"/>
-    <tableColumn id="3" name="Reviewer" dataDxfId="6"/>
-    <tableColumn id="4" name="Version" dataDxfId="5"/>
-    <tableColumn id="5" name="Review Comments" dataDxfId="4"/>
-    <tableColumn id="6" name="Actions" dataDxfId="3"/>
-    <tableColumn id="7" name="Owner" dataDxfId="2"/>
-    <tableColumn id="8" name="Owner Status" dataDxfId="1"/>
-    <tableColumn id="9" name="Reviewer verification" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{154D141F-D70B-42BC-A41E-539A28623C91}" name="date" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{4302D07D-1297-4A5D-8113-2317E944B040}" name="Review ID" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{FBF8D811-3328-47BA-BC1D-3D576EA1DAB6}" name="Reviewed Entity" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{18FF139E-B651-4240-BB94-D9B167C69A0B}" name="Reviewer" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{B63C6CDA-7136-454D-9369-ADF32D470B5E}" name="Version" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{A3F78CBF-8865-4A12-B192-C2D9A7E27A67}" name="Review Comments" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{F15DDF96-B3DE-490B-B5E1-EA2B8996F9B7}" name="Actions" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{CD6623E7-579E-4453-B3EF-FB2A474583B7}" name="Owner" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{E5418A75-71B3-4C99-955B-196E2C83D64E}" name="Owner Status" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{FFFAAB40-2BF2-4CDE-A704-8DB308BED7C4}" name="Reviewer verification" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -698,22 +730,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39D1DECC-CF93-47E4-94A2-AD404E424C77}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="36.5703125" customWidth="1"/>
+    <col min="1" max="1" width="25.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" customWidth="1"/>
+    <col min="3" max="3" width="36.5546875" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -727,7 +759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
@@ -742,43 +774,51 @@
         <v>45763</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9"/>
-    </row>
-    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="9">
+        <v>45765</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="9"/>
     </row>
-    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="9"/>
     </row>
-    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="9"/>
     </row>
-    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="9"/>
     </row>
-    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="9"/>
     </row>
-    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -793,35 +833,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{774AF0B9-8F49-46C8-8EB7-0F5E66F92113}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.77734375" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="43.7109375" customWidth="1"/>
-    <col min="6" max="6" width="39.85546875" customWidth="1"/>
-    <col min="7" max="7" width="32.7109375" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" customWidth="1"/>
-    <col min="9" max="9" width="19.5703125" customWidth="1"/>
+    <col min="5" max="5" width="6.88671875" customWidth="1"/>
+    <col min="6" max="6" width="39.88671875" customWidth="1"/>
+    <col min="7" max="7" width="32.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" customWidth="1"/>
+    <col min="9" max="9" width="19.5546875" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D1" t="s">
         <v>8</v>
@@ -845,13 +886,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="4" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="4" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <f>DATE(2025,4,16)</f>
         <v>45763</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>15</v>
@@ -860,32 +901,32 @@
         <v>25</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>3</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="1:11" s="3" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="3" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <f t="shared" ref="A3:A13" si="0">DATE(2025,4,16)</f>
         <v>45763</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>16</v>
@@ -894,32 +935,32 @@
         <v>25</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>3</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="K3"/>
     </row>
-    <row r="4" spans="1:11" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="3" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>17</v>
@@ -928,32 +969,32 @@
         <v>25</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="K4"/>
     </row>
-    <row r="5" spans="1:11" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="3" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>18</v>
@@ -962,32 +1003,32 @@
         <v>25</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>3</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="K5"/>
     </row>
-    <row r="6" spans="1:11" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="3" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>19</v>
@@ -996,32 +1037,32 @@
         <v>25</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>3</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="K6"/>
     </row>
-    <row r="7" spans="1:11" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="3" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>20</v>
@@ -1030,32 +1071,32 @@
         <v>25</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>3</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="K7"/>
     </row>
-    <row r="8" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>21</v>
@@ -1064,32 +1105,32 @@
         <v>25</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>3</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="K8"/>
     </row>
-    <row r="9" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>22</v>
@@ -1098,32 +1139,32 @@
         <v>25</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>3</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="K9"/>
     </row>
-    <row r="10" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>23</v>
@@ -1132,32 +1173,32 @@
         <v>25</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>3</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="K10"/>
     </row>
-    <row r="11" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>24</v>
@@ -1166,317 +1207,357 @@
         <v>25</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>3</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="K11"/>
     </row>
-    <row r="12" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>25</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>3</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>25</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>3</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="J13" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="9">
+        <v>45765</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="9">
+        <v>45765</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I15" s="7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="12"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="12"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="12"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="12"/>
+      <c r="J15" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="8"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H32:H1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H32:H1048576" xr:uid="{FDF361F9-8A76-4851-9C50-9A28BC1FE0CE}">
       <formula1>"open,inProgress,notApplicable,close"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I31" xr:uid="{7106F391-5C30-4C5F-9FBD-F7D4EC019822}">
       <formula1>"Open,InProgress,NotApplicable,Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J31" xr:uid="{A78E9E59-D51C-493A-A3EB-CA8CF067530D}">
       <formula1>"Open,Closed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
v1.2 Added reviews for the new version of the login testcases
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_TC_LOGIN_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_TC_LOGIN_REVIEWS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mego\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mego\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FEC51F6-FD26-411C-B8A9-22901276514B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3901E049-26F1-4FEE-A3B4-65F5CAC9BFA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5AC26BFC-4949-4339-B766-2ABB4B88E1A8}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="81">
   <si>
     <t>Author</t>
   </si>
@@ -234,13 +234,7 @@
 2-Remove the word SHEET from the name</t>
   </si>
   <si>
-    <t>LH_REVIEW_TC_LOGIN_014</t>
-  </si>
-  <si>
     <t>Closed</t>
-  </si>
-  <si>
-    <t>1-There is no status and Acutual results column which are necessary for tc execution</t>
   </si>
   <si>
     <t>1-user is already registered precondition is unnecessary
@@ -248,13 +242,68 @@
 3-in the steps column steps index number is mixed with the steps data because there are no spaces, bad redability</t>
   </si>
   <si>
+    <t>LH_REVIEW_TC_LOGIN_014</t>
+  </si>
+  <si>
     <t>Status column
 and Acutal results
 column</t>
   </si>
   <si>
+    <t>1.1</t>
+  </si>
+  <si>
     <t>1-Add Status column with 4 choices
 Pass,Fail,Blocked,Not executed and the default placeholder is Not executed</t>
+  </si>
+  <si>
+    <t>LH_REVIEW_TC_LOGIN_015</t>
+  </si>
+  <si>
+    <t>LH_REVIEW_TC_LOGIN_016</t>
+  </si>
+  <si>
+    <t>LH_REVIEW_TC_LOGIN_017</t>
+  </si>
+  <si>
+    <t>LH_REVIEW_TC_LOGIN_018</t>
+  </si>
+  <si>
+    <t>LH_REVIEW_TC_LOGIN_019</t>
+  </si>
+  <si>
+    <t>1-Test Data for login is Username and password and the user can only login using E-mail and password</t>
+  </si>
+  <si>
+    <t>1-Change the Username to E-mail</t>
+  </si>
+  <si>
+    <t>1-Test Data for login is Username and password and the user can only login using E-mail and password
+2-The username(email) provided is an invalid 
+E-mail for the front-end validation only and there is no testcase covering the invalid
+E-mail( an email that is not registered)</t>
+  </si>
+  <si>
+    <t>v1.2</t>
+  </si>
+  <si>
+    <t>1-Test Data for login is Username and password and the user can only login using E-mail and password
+2- Testcase testing wrong password should include a Valid E-mail and this tc has invalid 
+E-mail</t>
+  </si>
+  <si>
+    <t>1-Change the Username to E-mail
+2-Create a testcase with an invalid E-mail in the correct email form to bypass front-end validation eg:(invalidemail@gmail.com)</t>
+  </si>
+  <si>
+    <t>1-Change the Username to E-mail
+2-Use Valid email for this Testcase since the user is already registered is a precondition</t>
+  </si>
+  <si>
+    <t>Added reviews for the new version of the Testcases file</t>
+  </si>
+  <si>
+    <t>1-There is no status and Acutual results column which are necessary for tc execution</t>
   </si>
   <si>
     <t>Added crucial missing review points regarding the TC_ID column and modified Filename review and Status and Actual result column</t>
@@ -734,7 +783,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -782,17 +831,25 @@
         <v>25</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="D3" s="9">
         <v>45765</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="9"/>
+    <row r="4" spans="1:4" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="9">
+        <v>45766</v>
+      </c>
     </row>
     <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
@@ -836,8 +893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{774AF0B9-8F49-46C8-8EB7-0F5E66F92113}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -846,12 +903,12 @@
     <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.77734375" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="6.88671875" customWidth="1"/>
+    <col min="5" max="5" width="8.21875" customWidth="1"/>
     <col min="6" max="6" width="39.88671875" customWidth="1"/>
     <col min="7" max="7" width="32.6640625" customWidth="1"/>
     <col min="8" max="8" width="13.33203125" customWidth="1"/>
     <col min="9" max="9" width="19.5546875" customWidth="1"/>
-    <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="10" max="10" width="20.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -913,10 +970,10 @@
         <v>3</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K2" s="5"/>
     </row>
@@ -938,7 +995,7 @@
         <v>47</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>31</v>
@@ -947,10 +1004,10 @@
         <v>3</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K3"/>
     </row>
@@ -981,10 +1038,10 @@
         <v>3</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K4"/>
     </row>
@@ -1015,10 +1072,10 @@
         <v>3</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K5"/>
     </row>
@@ -1049,10 +1106,10 @@
         <v>3</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K6"/>
     </row>
@@ -1083,10 +1140,10 @@
         <v>3</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K7"/>
     </row>
@@ -1117,10 +1174,10 @@
         <v>3</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K8"/>
     </row>
@@ -1151,10 +1208,10 @@
         <v>3</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K9"/>
     </row>
@@ -1185,10 +1242,10 @@
         <v>3</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K10"/>
     </row>
@@ -1219,10 +1276,10 @@
         <v>3</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K11"/>
     </row>
@@ -1253,10 +1310,10 @@
         <v>3</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -1286,10 +1343,10 @@
         <v>3</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
@@ -1318,10 +1375,10 @@
         <v>3</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
@@ -1329,10 +1386,10 @@
         <v>45765</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>25</v>
@@ -1341,7 +1398,7 @@
         <v>47</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>65</v>
@@ -1349,72 +1406,172 @@
       <c r="H15" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I15" s="7" t="s">
+      <c r="I15" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="J15" s="7" t="s">
+      <c r="J15" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
+    <row r="16" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="9">
+        <v>45766</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="9">
+        <v>45766</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A18" s="9">
+        <v>45766</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="9">
+        <v>45766</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="9">
+        <v>45766</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="8"/>

</xml_diff>

<commit_message>
V1.3 Set Owner Status to closed
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_TC_LOGIN_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_TC_LOGIN_REVIEWS.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mego\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halae\OneDrive\Documents\GitHub\Group-3-Learning-hub\LH_REVIEWS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3901E049-26F1-4FEE-A3B4-65F5CAC9BFA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5AC26BFC-4949-4339-B766-2ABB4B88E1A8}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="Version History" sheetId="1" r:id="rId1"/>
     <sheet name="Review sheet" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="83">
   <si>
     <t>Author</t>
   </si>
@@ -308,11 +307,17 @@
   <si>
     <t>Added crucial missing review points regarding the TC_ID column and modified Filename review and Status and Actual result column</t>
   </si>
+  <si>
+    <t>Set Owner Status to closed</t>
+  </si>
+  <si>
+    <t>v1.3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -452,12 +457,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{83973D6D-C4A2-4DA6-8E86-0E47BD1D4D6C}" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{55AF0159-5A5D-4FB8-B45C-3CCBCD52D82E}" name="Version Number" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{A1BB0B96-5946-458D-A1EB-D1860A2E9A2C}" name="Author" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{7757C6A1-AD9C-489D-82AA-BCA0AEDC7F50}" name="Updated Section" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{484250C4-2243-4A67-B67B-4A70A88C9D78}" name="Date" dataDxfId="11">
+    <tableColumn id="1" name="Version Number" dataDxfId="14"/>
+    <tableColumn id="2" name="Author" dataDxfId="13"/>
+    <tableColumn id="3" name="Updated Section" dataDxfId="12"/>
+    <tableColumn id="4" name="Date" dataDxfId="11">
       <calculatedColumnFormula>DATE(2025,4,16)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -466,18 +471,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{24F4B5B1-870D-49D9-886C-D18ECE106044}" name="Table2" displayName="Table2" ref="A1:J31" totalsRowShown="0" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J31" totalsRowShown="0" dataDxfId="10">
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{154D141F-D70B-42BC-A41E-539A28623C91}" name="date" dataDxfId="9"/>
-    <tableColumn id="11" xr3:uid="{4302D07D-1297-4A5D-8113-2317E944B040}" name="Review ID" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{FBF8D811-3328-47BA-BC1D-3D576EA1DAB6}" name="Reviewed Entity" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{18FF139E-B651-4240-BB94-D9B167C69A0B}" name="Reviewer" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{B63C6CDA-7136-454D-9369-ADF32D470B5E}" name="Version" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{A3F78CBF-8865-4A12-B192-C2D9A7E27A67}" name="Review Comments" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{F15DDF96-B3DE-490B-B5E1-EA2B8996F9B7}" name="Actions" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{CD6623E7-579E-4453-B3EF-FB2A474583B7}" name="Owner" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{E5418A75-71B3-4C99-955B-196E2C83D64E}" name="Owner Status" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{FFFAAB40-2BF2-4CDE-A704-8DB308BED7C4}" name="Reviewer verification" dataDxfId="0"/>
+    <tableColumn id="1" name="date" dataDxfId="9"/>
+    <tableColumn id="11" name="Review ID" dataDxfId="8"/>
+    <tableColumn id="2" name="Reviewed Entity" dataDxfId="7"/>
+    <tableColumn id="3" name="Reviewer" dataDxfId="6"/>
+    <tableColumn id="4" name="Version" dataDxfId="5"/>
+    <tableColumn id="5" name="Review Comments" dataDxfId="4"/>
+    <tableColumn id="6" name="Actions" dataDxfId="3"/>
+    <tableColumn id="7" name="Owner" dataDxfId="2"/>
+    <tableColumn id="8" name="Owner Status" dataDxfId="1"/>
+    <tableColumn id="9" name="Reviewer verification" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -779,22 +784,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39D1DECC-CF93-47E4-94A2-AD404E424C77}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.109375" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" customWidth="1"/>
-    <col min="3" max="3" width="36.5546875" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="36.5703125" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -808,7 +813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
@@ -823,7 +828,7 @@
         <v>45763</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>57</v>
       </c>
@@ -837,7 +842,7 @@
         <v>45765</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>74</v>
       </c>
@@ -851,31 +856,39 @@
         <v>45766</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9"/>
-    </row>
-    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="9">
+        <v>45768</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="9"/>
     </row>
-    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="9"/>
     </row>
-    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="9"/>
     </row>
-    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -890,28 +903,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{774AF0B9-8F49-46C8-8EB7-0F5E66F92113}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="8.21875" customWidth="1"/>
-    <col min="6" max="6" width="39.88671875" customWidth="1"/>
-    <col min="7" max="7" width="32.6640625" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" customWidth="1"/>
-    <col min="9" max="9" width="19.5546875" customWidth="1"/>
-    <col min="10" max="10" width="20.5546875" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" customWidth="1"/>
+    <col min="6" max="6" width="39.85546875" customWidth="1"/>
+    <col min="7" max="7" width="32.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" customWidth="1"/>
+    <col min="10" max="10" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -943,7 +956,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="4" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="4" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <f>DATE(2025,4,16)</f>
         <v>45763</v>
@@ -977,7 +990,7 @@
       </c>
       <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="1:11" s="3" customFormat="1" ht="144" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" s="3" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <f t="shared" ref="A3:A13" si="0">DATE(2025,4,16)</f>
         <v>45763</v>
@@ -1011,7 +1024,7 @@
       </c>
       <c r="K3"/>
     </row>
-    <row r="4" spans="1:11" s="3" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
@@ -1045,7 +1058,7 @@
       </c>
       <c r="K4"/>
     </row>
-    <row r="5" spans="1:11" s="3" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
@@ -1079,7 +1092,7 @@
       </c>
       <c r="K5"/>
     </row>
-    <row r="6" spans="1:11" s="3" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
@@ -1113,7 +1126,7 @@
       </c>
       <c r="K6"/>
     </row>
-    <row r="7" spans="1:11" s="3" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
@@ -1147,7 +1160,7 @@
       </c>
       <c r="K7"/>
     </row>
-    <row r="8" spans="1:11" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
@@ -1181,7 +1194,7 @@
       </c>
       <c r="K8"/>
     </row>
-    <row r="9" spans="1:11" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
@@ -1215,7 +1228,7 @@
       </c>
       <c r="K9"/>
     </row>
-    <row r="10" spans="1:11" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
@@ -1249,7 +1262,7 @@
       </c>
       <c r="K10"/>
     </row>
-    <row r="11" spans="1:11" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
@@ -1283,7 +1296,7 @@
       </c>
       <c r="K11"/>
     </row>
-    <row r="12" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
@@ -1316,7 +1329,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
@@ -1349,7 +1362,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>45765</v>
       </c>
@@ -1381,7 +1394,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>45765</v>
       </c>
@@ -1407,13 +1420,13 @@
         <v>3</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="J15" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>45766</v>
       </c>
@@ -1439,13 +1452,13 @@
         <v>3</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="J16" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>45766</v>
       </c>
@@ -1471,13 +1484,13 @@
         <v>3</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="J17" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>45766</v>
       </c>
@@ -1503,13 +1516,13 @@
         <v>3</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="J18" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>45766</v>
       </c>
@@ -1535,13 +1548,13 @@
         <v>3</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="J19" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>45766</v>
       </c>
@@ -1567,13 +1580,13 @@
         <v>3</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="J20" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -1585,7 +1598,7 @@
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -1597,7 +1610,7 @@
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -1609,7 +1622,7 @@
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -1621,7 +1634,7 @@
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -1633,7 +1646,7 @@
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -1645,7 +1658,7 @@
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
@@ -1657,7 +1670,7 @@
       <c r="I27" s="8"/>
       <c r="J27" s="8"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
@@ -1669,7 +1682,7 @@
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
@@ -1681,7 +1694,7 @@
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -1693,7 +1706,7 @@
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
@@ -1708,13 +1721,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H32:H1048576" xr:uid="{FDF361F9-8A76-4851-9C50-9A28BC1FE0CE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H32:H1048576">
       <formula1>"open,inProgress,notApplicable,close"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I31" xr:uid="{7106F391-5C30-4C5F-9FBD-F7D4EC019822}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I31">
       <formula1>"Open,InProgress,NotApplicable,Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J31" xr:uid="{A78E9E59-D51C-493A-A3EB-CA8CF067530D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J31">
       <formula1>"Open,Closed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
v1.4 Set reviewer verification to closed
LH_TC_LOGIN_Review_004
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_TC_LOGIN_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_TC_LOGIN_REVIEWS.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halae\OneDrive\Documents\GitHub\Group-3-Learning-hub\LH_REVIEWS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mego\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE66EDD-1EC0-42FF-ACC8-36C06E9249E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version History" sheetId="1" r:id="rId1"/>
     <sheet name="Review sheet" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="84">
   <si>
     <t>Author</t>
   </si>
@@ -114,9 +115,6 @@
   </si>
   <si>
     <t>Mahmoud abdelmageed</t>
-  </si>
-  <si>
-    <t>Open</t>
   </si>
   <si>
     <t>1-there is no space between the username and the password in the test data column 
@@ -313,11 +311,17 @@
   <si>
     <t>v1.3</t>
   </si>
+  <si>
+    <t>v1.4</t>
+  </si>
+  <si>
+    <t>Set Reviewer verification to closed</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -457,12 +461,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <tableColumns count="4">
-    <tableColumn id="1" name="Version Number" dataDxfId="14"/>
-    <tableColumn id="2" name="Author" dataDxfId="13"/>
-    <tableColumn id="3" name="Updated Section" dataDxfId="12"/>
-    <tableColumn id="4" name="Date" dataDxfId="11">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Version Number" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Author" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Updated Section" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Date" dataDxfId="11">
       <calculatedColumnFormula>DATE(2025,4,16)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -471,18 +475,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J31" totalsRowShown="0" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:J31" totalsRowShown="0" dataDxfId="10">
   <tableColumns count="10">
-    <tableColumn id="1" name="date" dataDxfId="9"/>
-    <tableColumn id="11" name="Review ID" dataDxfId="8"/>
-    <tableColumn id="2" name="Reviewed Entity" dataDxfId="7"/>
-    <tableColumn id="3" name="Reviewer" dataDxfId="6"/>
-    <tableColumn id="4" name="Version" dataDxfId="5"/>
-    <tableColumn id="5" name="Review Comments" dataDxfId="4"/>
-    <tableColumn id="6" name="Actions" dataDxfId="3"/>
-    <tableColumn id="7" name="Owner" dataDxfId="2"/>
-    <tableColumn id="8" name="Owner Status" dataDxfId="1"/>
-    <tableColumn id="9" name="Reviewer verification" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="date" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Review ID" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Reviewed Entity" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Reviewer" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Version" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Review Comments" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Actions" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Owner" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Owner Status" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Reviewer verification" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -784,22 +788,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="36.5703125" customWidth="1"/>
+    <col min="1" max="1" width="25.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" customWidth="1"/>
+    <col min="3" max="3" width="36.5546875" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -813,7 +817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
@@ -828,67 +832,75 @@
         <v>45763</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D3" s="9">
         <v>45765</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D4" s="9">
         <v>45766</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D5" s="9">
         <v>45768</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="9"/>
-    </row>
-    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="9">
+        <v>45770</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="9"/>
     </row>
-    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="9"/>
     </row>
-    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -903,36 +915,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" customWidth="1"/>
-    <col min="6" max="6" width="39.85546875" customWidth="1"/>
-    <col min="7" max="7" width="32.7109375" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" customWidth="1"/>
-    <col min="9" max="9" width="19.5703125" customWidth="1"/>
-    <col min="10" max="10" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" customWidth="1"/>
+    <col min="6" max="6" width="39.88671875" customWidth="1"/>
+    <col min="7" max="7" width="32.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" customWidth="1"/>
+    <col min="9" max="9" width="19.5546875" customWidth="1"/>
+    <col min="10" max="10" width="20.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
         <v>34</v>
-      </c>
-      <c r="C1" t="s">
-        <v>35</v>
       </c>
       <c r="D1" t="s">
         <v>8</v>
@@ -956,13 +968,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="4" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="4" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <f>DATE(2025,4,16)</f>
         <v>45763</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>15</v>
@@ -971,32 +983,32 @@
         <v>25</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>30</v>
-      </c>
       <c r="H2" s="7" t="s">
         <v>3</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="1:11" s="3" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="3" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <f t="shared" ref="A3:A13" si="0">DATE(2025,4,16)</f>
         <v>45763</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>16</v>
@@ -1005,32 +1017,32 @@
         <v>25</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>3</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K3"/>
     </row>
-    <row r="4" spans="1:11" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="3" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>17</v>
@@ -1039,32 +1051,32 @@
         <v>25</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K4"/>
     </row>
-    <row r="5" spans="1:11" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="3" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>18</v>
@@ -1073,32 +1085,32 @@
         <v>25</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>3</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K5"/>
     </row>
-    <row r="6" spans="1:11" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="3" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>19</v>
@@ -1107,32 +1119,32 @@
         <v>25</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>3</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K6"/>
     </row>
-    <row r="7" spans="1:11" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="3" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>20</v>
@@ -1141,32 +1153,32 @@
         <v>25</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>3</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K7"/>
     </row>
-    <row r="8" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>21</v>
@@ -1175,32 +1187,32 @@
         <v>25</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>3</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K8"/>
     </row>
-    <row r="9" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>22</v>
@@ -1209,32 +1221,32 @@
         <v>25</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>3</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K9"/>
     </row>
-    <row r="10" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>23</v>
@@ -1243,32 +1255,32 @@
         <v>25</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>3</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K10"/>
     </row>
-    <row r="11" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>24</v>
@@ -1277,161 +1289,161 @@
         <v>25</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>3</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K11"/>
     </row>
-    <row r="12" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>47</v>
-      </c>
       <c r="F12" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="G12" s="7" t="s">
-        <v>59</v>
-      </c>
       <c r="H12" s="7" t="s">
         <v>3</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="D13" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>50</v>
-      </c>
       <c r="H13" s="7" t="s">
         <v>3</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>45765</v>
       </c>
       <c r="B14" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="D14" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>53</v>
-      </c>
       <c r="H14" s="7" t="s">
         <v>3</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>45765</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>63</v>
-      </c>
       <c r="D15" s="7" t="s">
         <v>25</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>3</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>45766</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>15</v>
@@ -1440,30 +1452,30 @@
         <v>25</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F16" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G16" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="G16" s="8" t="s">
-        <v>72</v>
-      </c>
       <c r="H16" s="7" t="s">
         <v>3</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
         <v>45766</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>16</v>
@@ -1472,30 +1484,30 @@
         <v>25</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H17" s="7" t="s">
         <v>3</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A18" s="9">
         <v>45766</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>17</v>
@@ -1504,30 +1516,30 @@
         <v>25</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>3</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
         <v>45766</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>18</v>
@@ -1536,30 +1548,30 @@
         <v>25</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F19" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G19" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="G19" s="8" t="s">
-        <v>72</v>
-      </c>
       <c r="H19" s="7" t="s">
         <v>3</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="9">
         <v>45766</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>20</v>
@@ -1568,25 +1580,25 @@
         <v>25</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F20" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G20" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="G20" s="8" t="s">
-        <v>72</v>
-      </c>
       <c r="H20" s="7" t="s">
         <v>3</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -1598,7 +1610,7 @@
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -1610,7 +1622,7 @@
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -1622,7 +1634,7 @@
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -1634,7 +1646,7 @@
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -1646,7 +1658,7 @@
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -1658,7 +1670,7 @@
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
@@ -1670,7 +1682,7 @@
       <c r="I27" s="8"/>
       <c r="J27" s="8"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
@@ -1682,7 +1694,7 @@
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
@@ -1694,7 +1706,7 @@
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -1706,7 +1718,7 @@
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
@@ -1721,13 +1733,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H32:H1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H32:H1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"open,inProgress,notApplicable,close"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I31" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Open,InProgress,NotApplicable,Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J31" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"Open,Closed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
v2.0 Review LOGIN and No comments
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_TC_LOGIN_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_TC_LOGIN_REVIEWS.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mego\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halae\OneDrive\Desktop\oooo\Group-3-Learning-hub-dev\LH_REVIEWS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE66EDD-1EC0-42FF-ACC8-36C06E9249E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="4080" windowHeight="6930"/>
   </bookViews>
   <sheets>
     <sheet name="Version History" sheetId="1" r:id="rId1"/>
     <sheet name="Review sheet" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="86">
   <si>
     <t>Author</t>
   </si>
@@ -317,11 +316,17 @@
   <si>
     <t>Set Reviewer verification to closed</t>
   </si>
+  <si>
+    <t>v2.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Comments </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -461,12 +466,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Version Number" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Author" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Updated Section" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Date" dataDxfId="11">
+    <tableColumn id="1" name="Version Number" dataDxfId="14"/>
+    <tableColumn id="2" name="Author" dataDxfId="13"/>
+    <tableColumn id="3" name="Updated Section" dataDxfId="12"/>
+    <tableColumn id="4" name="Date" dataDxfId="11">
       <calculatedColumnFormula>DATE(2025,4,16)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -475,18 +480,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:J31" totalsRowShown="0" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J31" totalsRowShown="0" dataDxfId="10">
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="date" dataDxfId="9"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Review ID" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Reviewed Entity" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Reviewer" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Version" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Review Comments" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Actions" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Owner" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Owner Status" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Reviewer verification" dataDxfId="0"/>
+    <tableColumn id="1" name="date" dataDxfId="9"/>
+    <tableColumn id="11" name="Review ID" dataDxfId="8"/>
+    <tableColumn id="2" name="Reviewed Entity" dataDxfId="7"/>
+    <tableColumn id="3" name="Reviewer" dataDxfId="6"/>
+    <tableColumn id="4" name="Version" dataDxfId="5"/>
+    <tableColumn id="5" name="Review Comments" dataDxfId="4"/>
+    <tableColumn id="6" name="Actions" dataDxfId="3"/>
+    <tableColumn id="7" name="Owner" dataDxfId="2"/>
+    <tableColumn id="8" name="Owner Status" dataDxfId="1"/>
+    <tableColumn id="9" name="Reviewer verification" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -788,22 +793,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.109375" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" customWidth="1"/>
-    <col min="3" max="3" width="36.5546875" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="36.5703125" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -817,7 +822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
@@ -832,7 +837,7 @@
         <v>45763</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>56</v>
       </c>
@@ -846,7 +851,7 @@
         <v>45765</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>73</v>
       </c>
@@ -860,7 +865,7 @@
         <v>45766</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>81</v>
       </c>
@@ -874,7 +879,7 @@
         <v>45768</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>82</v>
       </c>
@@ -888,19 +893,27 @@
         <v>45770</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9"/>
-    </row>
-    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="9">
+        <v>45790</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="9"/>
     </row>
-    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -915,28 +928,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" customWidth="1"/>
-    <col min="6" max="6" width="39.88671875" customWidth="1"/>
-    <col min="7" max="7" width="32.6640625" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" customWidth="1"/>
-    <col min="9" max="9" width="19.5546875" customWidth="1"/>
-    <col min="10" max="10" width="20.5546875" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" customWidth="1"/>
+    <col min="6" max="6" width="39.85546875" customWidth="1"/>
+    <col min="7" max="7" width="32.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" customWidth="1"/>
+    <col min="10" max="10" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -968,7 +981,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="4" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="4" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <f>DATE(2025,4,16)</f>
         <v>45763</v>
@@ -1002,7 +1015,7 @@
       </c>
       <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="1:11" s="3" customFormat="1" ht="144" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" s="3" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <f t="shared" ref="A3:A13" si="0">DATE(2025,4,16)</f>
         <v>45763</v>
@@ -1036,7 +1049,7 @@
       </c>
       <c r="K3"/>
     </row>
-    <row r="4" spans="1:11" s="3" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
@@ -1070,7 +1083,7 @@
       </c>
       <c r="K4"/>
     </row>
-    <row r="5" spans="1:11" s="3" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
@@ -1104,7 +1117,7 @@
       </c>
       <c r="K5"/>
     </row>
-    <row r="6" spans="1:11" s="3" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
@@ -1138,7 +1151,7 @@
       </c>
       <c r="K6"/>
     </row>
-    <row r="7" spans="1:11" s="3" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
@@ -1172,7 +1185,7 @@
       </c>
       <c r="K7"/>
     </row>
-    <row r="8" spans="1:11" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
@@ -1206,7 +1219,7 @@
       </c>
       <c r="K8"/>
     </row>
-    <row r="9" spans="1:11" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
@@ -1240,7 +1253,7 @@
       </c>
       <c r="K9"/>
     </row>
-    <row r="10" spans="1:11" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
@@ -1274,7 +1287,7 @@
       </c>
       <c r="K10"/>
     </row>
-    <row r="11" spans="1:11" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
@@ -1308,7 +1321,7 @@
       </c>
       <c r="K11"/>
     </row>
-    <row r="12" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
@@ -1341,7 +1354,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <f t="shared" si="0"/>
         <v>45763</v>
@@ -1374,7 +1387,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>45765</v>
       </c>
@@ -1406,7 +1419,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>45765</v>
       </c>
@@ -1438,7 +1451,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>45766</v>
       </c>
@@ -1470,7 +1483,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>45766</v>
       </c>
@@ -1502,7 +1515,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>45766</v>
       </c>
@@ -1534,7 +1547,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>45766</v>
       </c>
@@ -1566,7 +1579,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>45766</v>
       </c>
@@ -1598,7 +1611,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -1610,7 +1623,7 @@
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -1622,7 +1635,7 @@
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -1634,7 +1647,7 @@
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -1646,7 +1659,7 @@
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -1658,7 +1671,7 @@
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -1670,7 +1683,7 @@
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
@@ -1682,7 +1695,7 @@
       <c r="I27" s="8"/>
       <c r="J27" s="8"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
@@ -1694,7 +1707,7 @@
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
@@ -1706,7 +1719,7 @@
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -1718,7 +1731,7 @@
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
@@ -1733,13 +1746,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H32:H1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H32:H1048576">
       <formula1>"open,inProgress,notApplicable,close"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I31" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I31">
       <formula1>"Open,InProgress,NotApplicable,Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J31" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J31">
       <formula1>"Open,Closed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>